<commit_message>
added file for printing out poster figures
</commit_message>
<xml_diff>
--- a/Final Iterations/f_bortozemib.xlsx
+++ b/Final Iterations/f_bortozemib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grollins/Desktop/CS/Capstone/Demyelination-Disease-Detection/Final Iterations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C3E70F-31C9-2647-A6B5-0D3F91370CFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C76ADB0-4FBC-7B4F-9C68-44849D72DA58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12726,7 +12726,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12771,7 +12771,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -12783,28 +12783,28 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2">
-        <v>0.66666666666666663</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="I2">
-        <v>0.63358778625954193</v>
+        <v>0.58536585365853655</v>
       </c>
       <c r="J2">
-        <v>0.79047619047619044</v>
+        <v>0.91428571428571426</v>
       </c>
       <c r="K2">
-        <v>0.70338983050847448</v>
+        <v>0.71375464684014878</v>
       </c>
       <c r="L2">
-        <v>0.52863636363636368</v>
+        <v>0.54863636363636359</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -12818,36 +12818,36 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3">
-        <v>0.61428571428571432</v>
+        <v>0.65238095238095239</v>
       </c>
       <c r="I3">
-        <v>0.5714285714285714</v>
+        <v>0.60810810810810811</v>
       </c>
       <c r="J3">
-        <v>0.91428571428571426</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="K3">
-        <v>0.70329670329670324</v>
+        <v>0.71146245059288538</v>
       </c>
       <c r="L3">
-        <v>0.58136363636363642</v>
+        <v>0.52772727272727271</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -12856,7 +12856,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -12868,19 +12868,19 @@
         <v>14</v>
       </c>
       <c r="H4">
-        <v>0.61428571428571432</v>
+        <v>0.62857142857142856</v>
       </c>
       <c r="I4">
-        <v>0.5714285714285714</v>
+        <v>0.58282208588957052</v>
       </c>
       <c r="J4">
-        <v>0.91428571428571426</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="K4">
-        <v>0.70329670329670324</v>
+        <v>0.70895522388059695</v>
       </c>
       <c r="L4">
-        <v>0.58636363636363642</v>
+        <v>0.57272727272727275</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -12888,16 +12888,16 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -12906,27 +12906,27 @@
         <v>13</v>
       </c>
       <c r="H5">
-        <v>0.65238095238095239</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I5">
-        <v>0.60810810810810811</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="J5">
-        <v>0.8571428571428571</v>
+        <v>0.8</v>
       </c>
       <c r="K5">
-        <v>0.71146245059288538</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="L5">
-        <v>0.52772727272727271</v>
+        <v>0.53363636363636369</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -12941,22 +12941,22 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6">
-        <v>0.66666666666666663</v>
+        <v>0.61904761904761907</v>
       </c>
       <c r="I6">
-        <v>0.63157894736842102</v>
+        <v>0.57485029940119758</v>
       </c>
       <c r="J6">
-        <v>0.8</v>
+        <v>0.91428571428571426</v>
       </c>
       <c r="K6">
-        <v>0.70588235294117652</v>
+        <v>0.70588235294117641</v>
       </c>
       <c r="L6">
-        <v>0.53363636363636369</v>
+        <v>0.57318181818181813</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -12967,10 +12967,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -12979,22 +12979,22 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7">
-        <v>0.65238095238095239</v>
+        <v>0.62380952380952381</v>
       </c>
       <c r="I7">
-        <v>0.61428571428571432</v>
+        <v>0.58024691358024694</v>
       </c>
       <c r="J7">
-        <v>0.81904761904761902</v>
+        <v>0.89523809523809528</v>
       </c>
       <c r="K7">
-        <v>0.70204081632653059</v>
+        <v>0.70411985018726597</v>
       </c>
       <c r="L7">
-        <v>0.66545454545454552</v>
+        <v>0.56818181818181812</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -13002,7 +13002,7 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -13023,13 +13023,13 @@
         <v>0.61904761904761907</v>
       </c>
       <c r="I8">
-        <v>0.57485029940119758</v>
+        <v>0.5757575757575758</v>
       </c>
       <c r="J8">
-        <v>0.91428571428571426</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="K8">
-        <v>0.70588235294117641</v>
+        <v>0.70370370370370383</v>
       </c>
       <c r="L8">
         <v>0.57318181818181813</v>
@@ -13037,7 +13037,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -13049,33 +13049,33 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9">
-        <v>0.6333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I9">
-        <v>0.58536585365853655</v>
+        <v>0.63358778625954193</v>
       </c>
       <c r="J9">
-        <v>0.91428571428571426</v>
+        <v>0.79047619047619044</v>
       </c>
       <c r="K9">
-        <v>0.71375464684014878</v>
+        <v>0.70338983050847448</v>
       </c>
       <c r="L9">
-        <v>0.54863636363636359</v>
+        <v>0.52863636363636368</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -13084,7 +13084,7 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -13096,24 +13096,24 @@
         <v>14</v>
       </c>
       <c r="H10">
-        <v>0.62380952380952381</v>
+        <v>0.61428571428571432</v>
       </c>
       <c r="I10">
-        <v>0.58024691358024694</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J10">
-        <v>0.89523809523809528</v>
+        <v>0.91428571428571426</v>
       </c>
       <c r="K10">
-        <v>0.70411985018726597</v>
+        <v>0.70329670329670324</v>
       </c>
       <c r="L10">
-        <v>0.56818181818181812</v>
+        <v>0.58136363636363642</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -13122,7 +13122,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -13134,19 +13134,19 @@
         <v>14</v>
       </c>
       <c r="H11">
-        <v>0.62857142857142856</v>
+        <v>0.61428571428571432</v>
       </c>
       <c r="I11">
-        <v>0.58282208588957052</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J11">
-        <v>0.90476190476190477</v>
+        <v>0.91428571428571426</v>
       </c>
       <c r="K11">
-        <v>0.70895522388059695</v>
+        <v>0.70329670329670324</v>
       </c>
       <c r="L11">
-        <v>0.57272727272727275</v>
+        <v>0.58636363636363642</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -13154,10 +13154,10 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -13169,22 +13169,22 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12">
-        <v>0.61904761904761907</v>
+        <v>0.65238095238095239</v>
       </c>
       <c r="I12">
-        <v>0.5757575757575758</v>
+        <v>0.61428571428571432</v>
       </c>
       <c r="J12">
-        <v>0.90476190476190477</v>
+        <v>0.81904761904761902</v>
       </c>
       <c r="K12">
-        <v>0.70370370370370383</v>
+        <v>0.70204081632653059</v>
       </c>
       <c r="L12">
-        <v>0.57318181818181813</v>
+        <v>0.66545454545454552</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -13264,6 +13264,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L14">
+    <sortCondition descending="1" ref="K2:K14"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>